<commit_message>
tweak(Sales): update invoice timesheet export template
* duration and sum values fix (minutes -> hours)

Change-Id: I7991411293f97bd914c393d4d98de5520026d2de
Reviewed-on: http://gerrit.tine20.com/customers/12059
Reviewed-by: Philipp Schüle <p.schuele@metaways.de>
Tested-by: Philipp Schüle <p.schuele@metaways.de>
</commit_message>
<xml_diff>
--- a/tine20/Sales/Export/templates/sales_invoice_timesheet.xlsx
+++ b/tine20/Sales/Export/templates/sales_invoice_timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mspahn/Workspace/tine20.com/tine20/Sales/Export/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pzornsch/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C41291-3E21-A448-AE9F-44FB10507C45}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE7AC20-AB73-0A49-B4FB-CA9D2B108C4C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25060" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheets" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Timesheets!$A$1:$H$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Timesheets!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -62,9 +70,6 @@
     <t>${twig:record.description}</t>
   </si>
   <si>
-    <t>${twig:record.duration}</t>
-  </si>
-  <si>
     <t>${twig:record.start_time}</t>
   </si>
   <si>
@@ -74,12 +79,6 @@
     <t>${twig:renderTags(record.tags)}${/ROW}</t>
   </si>
   <si>
-    <t>${twig:sum}</t>
-  </si>
-  <si>
-    <t>${twig:sumTag}</t>
-  </si>
-  <si>
     <t>${ROW}${twig:dateFormat(record.start_date,'date')}</t>
   </si>
   <si>
@@ -102,6 +101,15 @@
   </si>
   <si>
     <t>${twig:timeaccount.title}</t>
+  </si>
+  <si>
+    <t>${twig:record.duration/60}</t>
+  </si>
+  <si>
+    <t>${twig:sumTag/60}</t>
+  </si>
+  <si>
+    <t>${twig:sum/60}</t>
   </si>
 </sst>
 </file>
@@ -469,9 +477,9 @@
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -487,7 +495,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -785,9 +793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -807,10 +813,10 @@
     <row r="1" spans="1:12" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20"/>
       <c r="B1" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="17"/>
@@ -819,7 +825,7 @@
         <v>10</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -829,10 +835,10 @@
     <row r="2" spans="1:12" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="B2" s="16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="19"/>
@@ -882,28 +888,28 @@
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E5" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>13</v>
-      </c>
       <c r="H5" s="35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -914,7 +920,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
@@ -928,7 +934,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>

</xml_diff>